<commit_message>
pass 4 tc heap
</commit_message>
<xml_diff>
--- a/initial-BTL2/TestResult.xlsx
+++ b/initial-BTL2/TestResult.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\DSA-242-Khoa\initial-BTL2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958BACB0-6EE5-437A-BC4E-EBDF63B45617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EF0570-2DAC-42FD-95BD-640F5C38868E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5CCED45E-E3BF-48A3-AB89-CCCD024A6D56}"/>
+    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5CCED45E-E3BF-48A3-AB89-CCCD024A6D56}"/>
   </bookViews>
   <sheets>
     <sheet name="hashDemo" sheetId="1" r:id="rId1"/>
+    <sheet name="heapDemo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="187">
   <si>
     <t>Test</t>
   </si>
@@ -409,6 +410,189 @@
   </si>
   <si>
     <t>    cout &lt;&lt; "After clear:" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>void heapDemo1(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int array[] = {50, 20, 15, 10, 8, 6, 7, 23};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //min heap: [6, 10, 7, 23, 15, 20, 8, 50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //max heap: [50, 23, 15, 20, 8, 6, 7, 10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;int&gt; minHeap1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Min Heap: ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    minHeap1.heapify(array, 8);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; minHeap1.toString() &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;int&gt; minHeap2(minHeapComparator);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    minHeap2.heapify(array, 8);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; minHeap2.toString() &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;int&gt; maxHeap(maxHeapComparator);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Max Heap: ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    maxHeap.heapify(array, 8);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; maxHeap.toString() &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>Min Heap: [6,8,7,10,20,15,50,23]</t>
+  </si>
+  <si>
+    <t>Max Heap: [50,23,15,20,8,6,7,10]</t>
+  </si>
+  <si>
+    <t>void heapDemo2(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Point array[] = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Point(13.1, 12.4), Point(5.5, 4.5), Point(15.5, 14.5),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Point(23.1, 12.4), Point(35.5, 14.5), Point(5.5, 34.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;Point&gt; minHeap1(minHeapComparator);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    minHeap1.heapify(array, 6);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; minHeap1.toString(&amp;point2str) &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;Point&gt; maxHeap(maxHeapComparator);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    maxHeap.heapify(array, 6);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; maxHeap.toString(&amp;point2str) &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>Min Heap: [(5.5, 4.5),(13.1, 12.4),(15.5, 14.5),(23.1, 12.4),(35.5, 14.5),(5.5, 34.5)]</t>
+  </si>
+  <si>
+    <t>Max Heap: [(35.5, 14.5),(23.1, 12.4),(5.5, 34.5),(13.1, 12.4),(5.5, 4.5),(15.5, 14.5)]</t>
+  </si>
+  <si>
+    <t>void heapDemo3(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Point* array[] = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        new Point(13.1, 12.4), new Point(5.5, 4.5), new Point(15.5, 14.5),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        new Point(23.1, 12.4), new Point(35.5, 14.5), new Point(5.5, 34.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;Point*&gt; heap(&amp;myPointComparatorMAX, &amp;Heap&lt;Point*&gt;::free);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for(int idx=0; idx &lt; 6; idx++) heap.push(array[idx]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    heap.println(&amp;myPoint2Str);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for(Heap&lt;Point*&gt;::Iterator it = heap.begin(); it != heap.end(); it++){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Point* point = *it;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cout &lt;&lt; point-&gt;radius() &lt;&lt; ", ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>[[    36,     14],[    23,     12],[   5.5,     34],[   5.5,    4.5],[    16,     14],[    13,     12]]</t>
+  </si>
+  <si>
+    <t>38.3471, 26.2177, 34.9357, 7.10634, 21.225, 18.038,</t>
+  </si>
+  <si>
+    <t>void heapDemo4(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    XArrayList&lt;int&gt; list;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int values[] = {3, 1, 4, 1, 5, 9, 2, 6, 5};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int v : values) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        list.add(v);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Before heapsort: ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    list.println();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Heap&lt;int&gt; heap;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    heap.heapsort(list);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "After heapsort: ";</t>
+  </si>
+  <si>
+    <t>Before heapsort: [3, 1, 4, 1, 5, 9, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 4, 1, 5, 9, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 1, 5, 9, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 3, 5, 9, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 3, 4, 9, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 3, 4, 5, 2, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 3, 4, 5, 5, 6, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 3, 4, 5, 5, 6, 9]</t>
+  </si>
+  <si>
+    <t>After heapsort: [1, 1, 2, 3, 4, 5, 5, 6, 9]</t>
   </si>
 </sst>
 </file>
@@ -455,7 +639,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,8 +652,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -477,11 +667,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB0B0B0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB0B0B0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFB0B0B0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB0B0B0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB0B0B0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB0B0B0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB0B0B0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFB0B0B0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -516,6 +743,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,6 +1262,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3534268</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>143001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDB5257-DAD4-4916-A291-49A948DD454D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10753725" y="533400"/>
+          <a:ext cx="3534268" cy="905001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>534252</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A69E9EC-5A34-4C27-8C7D-CFE6817754E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10753725" y="4733925"/>
+          <a:ext cx="6106377" cy="819264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1322,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69154D13-923D-4E9F-9186-615A4A4601DE}">
   <dimension ref="A1:C208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+    <sheetView topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="A236" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,4 +2816,866 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6D0577-1287-497A-9FA6-80D309DD045A}">
+  <dimension ref="A1:C193"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="91.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
+      <c r="B67" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6"/>
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="6"/>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="6"/>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="6"/>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="6"/>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="6"/>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6"/>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6"/>
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="6"/>
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="6"/>
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="6"/>
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6"/>
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="6"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="6"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="6"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="6"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="6"/>
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="6"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="6"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="6"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="6"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="6"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="6"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="6"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="6"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="6"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="6"/>
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="6"/>
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="6"/>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="6"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="6"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="6"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="6"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="6"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="6"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="6"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="6"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="6"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="6"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="8"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="6"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="6"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="6"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="6"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="6"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="6"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="6"/>
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="6"/>
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="6"/>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="6"/>
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="6"/>
+      <c r="B155" s="2"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="6"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="6"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="6"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="6"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="6"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="6"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="6"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="6"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="6"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="6"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="6"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="8"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="6"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="6"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="9"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="9"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="9"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="9"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="9"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="9"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="9"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="9"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="9"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="9"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="9"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="9"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="9"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="9"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="9"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="9"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="9"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="11"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pass 3 tc huffman
</commit_message>
<xml_diff>
--- a/initial-BTL2/TestResult.xlsx
+++ b/initial-BTL2/TestResult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\DSA-242-Khoa\initial-BTL2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCDE98B-66AE-4CF1-89B2-470251F93539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A3E3CC-3B50-4469-99EC-61D708745885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5CCED45E-E3BF-48A3-AB89-CCCD024A6D56}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="246">
   <si>
     <t>Test</t>
   </si>
@@ -594,6 +594,183 @@
   </si>
   <si>
     <t>After heapsort: [1, 1, 2, 3, 4, 5, 5, 6, 9]</t>
+  </si>
+  <si>
+    <t>void tc_huffman1001() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    XArrayList&lt;pair&lt;char, int&gt;&gt; symbolFreqs;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('A', 5));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('B', 3));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    HTree tree;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    tree.build(symbolFreqs);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    xMap&lt;char, string&gt; codeTable(&amp;charHashFunc);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    tree.generateCodes(codeTable);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string codeA = codeTable.get('A');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Code for A: " &lt;&lt; codeA &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string decoded = tree.decode(codeA);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Decoded string: " &lt;&lt; decoded &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>Code for A: 2</t>
+  </si>
+  <si>
+    <t>Decoded string: A</t>
+  </si>
+  <si>
+    <t>void tc_huffman1002() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('C', 7));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('D', 2));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Generated codes:" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (char ch = 'A'; ch &lt;= 'D'; ++ch) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        string code = codeTable.get(ch);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cout &lt;&lt; "Code for " &lt;&lt; ch &lt;&lt; ": " &lt;&lt; code &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>Generated codes:</t>
+  </si>
+  <si>
+    <t>Code for A: 0</t>
+  </si>
+  <si>
+    <t>Code for B: 12</t>
+  </si>
+  <si>
+    <t>Code for C: 2</t>
+  </si>
+  <si>
+    <t>Code for D: 11</t>
+  </si>
+  <si>
+    <t>void tc_huffman1003() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('X', 4));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('Y', 6));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('Z', 2));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string codeZ = codeTable.get('Z');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Code for Z: " &lt;&lt; codeZ &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string decoded = tree.decode(codeZ);</t>
+  </si>
+  <si>
+    <t>Code for Z: 0</t>
+  </si>
+  <si>
+    <t>Decoded string: Z</t>
+  </si>
+  <si>
+    <t>void tc_huffman1004() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('M', 3));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    symbolFreqs.add(make_pair('N', 5));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string decoded = tree.decode("0");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Decoded string from invalid code: " &lt;&lt; decoded &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>Decoded string from invalid code: \x00</t>
+  </si>
+  <si>
+    <t>void tc_huffman1005() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    const string symbols = "ABCDEFGHIJ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int n = symbols.size();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; i &lt; n; ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        symbolFreqs.add(make_pair(symbols[i], (i + 1) * 2));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (char ch : symbols) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        string decoded = tree.decode(code);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cout &lt;&lt; ch &lt;&lt; " with code " &lt;&lt; code &lt;&lt; " decodes as: " &lt;&lt; decoded &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>A with code 011 decodes as: A</t>
+  </si>
+  <si>
+    <t>B with code 012 decodes as: B</t>
+  </si>
+  <si>
+    <t>C with code 00 decodes as: C</t>
+  </si>
+  <si>
+    <t>D with code 02 decodes as: D</t>
+  </si>
+  <si>
+    <t>E with code 10 decodes as: E</t>
+  </si>
+  <si>
+    <t>F with code 11 decodes as: F</t>
+  </si>
+  <si>
+    <t>G with code 12 decodes as: G</t>
+  </si>
+  <si>
+    <t>H with code 20 decodes as: H</t>
+  </si>
+  <si>
+    <t>I with code 21 decodes as: I</t>
+  </si>
+  <si>
+    <t>J with code 22 decodes as: J</t>
   </si>
 </sst>
 </file>
@@ -640,7 +817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -656,6 +833,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5E5E5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -755,6 +938,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1356,6 +1551,231 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3581900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC434B2D-7010-4E07-972C-67D83107E04E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="342900"/>
+          <a:ext cx="3581900" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3686689</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>186</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA754B42-1A6A-4863-8168-C80BB2ECE055}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="3981450"/>
+          <a:ext cx="3686689" cy="1333686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3962953</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19186</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEAE5E56-DE5F-447B-A0B6-8855EFFC4917}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="7991475"/>
+          <a:ext cx="3962953" cy="971686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4553585</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>114396</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4897D1DE-49FF-4194-99A5-8B40DEB1FB23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="11610975"/>
+          <a:ext cx="4553585" cy="685896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4467849</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>105082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B6CA2F-A293-430C-BAF5-5022D47D583D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12058650" y="14468475"/>
+          <a:ext cx="4467849" cy="2200582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3685,8 +4105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4F783D-4D66-477B-8663-19EF23D56317}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,7 +4116,7 @@
     <col min="3" max="3" width="80.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3708,156 +4128,230 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="18" t="s">
+        <v>188</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="18" t="s">
+        <v>190</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="18" t="s">
+        <v>192</v>
+      </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="18" t="s">
+        <v>193</v>
+      </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="18" t="s">
+        <v>194</v>
+      </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="18" t="s">
+        <v>195</v>
+      </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="18" t="s">
+        <v>196</v>
+      </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="18" t="s">
+        <v>197</v>
+      </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="18" t="s">
+        <v>198</v>
+      </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="14" t="s">
+        <v>191</v>
+      </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="A30" s="14" t="s">
+        <v>192</v>
+      </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="14" t="s">
+        <v>194</v>
+      </c>
       <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="14" t="s">
+        <v>204</v>
+      </c>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="A36" s="14" t="s">
+        <v>205</v>
+      </c>
       <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="A37" s="14" t="s">
+        <v>206</v>
+      </c>
       <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="14" t="s">
+        <v>207</v>
+      </c>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="A39" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
     </row>
@@ -3867,74 +4361,108 @@
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
+      <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+      <c r="A48" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
+      <c r="A50" s="1"/>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
+      <c r="A51" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
+      <c r="A52" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+      <c r="A53" s="1"/>
       <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+      <c r="A54" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
+      <c r="A55" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
@@ -3944,65 +4472,89 @@
       <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
+      <c r="A62" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
+      <c r="A63" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+      <c r="A64" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+      <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
+      <c r="A67" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
+      <c r="A68" s="1"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
+      <c r="A69" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
+      <c r="A70" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
+      <c r="A71" s="1"/>
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
+      <c r="A72" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+      <c r="A73" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4010,80 +4562,135 @@
       <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="3"/>
+      <c r="A76" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3"/>
+      <c r="A77" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
+      <c r="A78" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
+      <c r="A79" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
+      <c r="A80" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
+      <c r="A81" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
+      <c r="A82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
+      <c r="A83" s="1"/>
+      <c r="B83" s="2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
+      <c r="A84" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
+      <c r="A85" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
+      <c r="A86" s="1"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
+      <c r="A87" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
+      <c r="A88" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="B88" s="2"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="6"/>
+      <c r="A89" s="1"/>
       <c r="B89" s="2"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
+      <c r="A90" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
+      <c r="A91" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="6"/>
+      <c r="A92" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
+      <c r="A93" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
+      <c r="A94" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="6"/>
+      <c r="A95" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -4132,5 +4739,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>